<commit_message>
Falta corregir el xlsx modificado
</commit_message>
<xml_diff>
--- a/EmpleadosConSalarios.xlsx
+++ b/EmpleadosConSalarios.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="Rc367c26adb1c4807"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="Rfeb239e55142497a"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <x:si>
     <x:t>Nombre</x:t>
   </x:si>
@@ -35,22 +35,19 @@
     <x:t>Salario</x:t>
   </x:si>
   <x:si>
-    <x:t>Felipe</x:t>
+    <x:t>Julian</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PROGRAMADOR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Juan</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Alexis </x:t>
   </x:si>
   <x:si>
     <x:t>ANALISTA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Julian</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PROGRAMADOR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Juan</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Alexis </x:t>
   </x:si>
 </x:sst>
 </file>
@@ -381,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:G5"/>
+  <x:dimension ref="A1:G6"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -415,27 +412,27 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B2">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>1000</x:v>
+        <x:v>1200</x:v>
       </x:c>
       <x:c r="D2">
-        <x:v>40</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E2">
-        <x:v>4</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F2" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="G2">
-        <x:v>44000</x:v>
+        <x:v>43200</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="A3" t="s">
-        <x:v>9</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B3">
         <x:v>19</x:v>
@@ -450,7 +447,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="F3" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G3">
         <x:v>43200</x:v>
@@ -458,7 +455,7 @@
     </x:row>
     <x:row r="4">
       <x:c r="A4" t="s">
-        <x:v>11</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B4">
         <x:v>20</x:v>
@@ -473,7 +470,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="F4" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G4">
         <x:v>48000</x:v>
@@ -481,24 +478,47 @@
     </x:row>
     <x:row r="5">
       <x:c r="A5" t="s">
-        <x:v>12</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B5">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>1000</x:v>
+        <x:v>1200</x:v>
       </x:c>
       <x:c r="D5">
         <x:v>40</x:v>
       </x:c>
       <x:c r="E5">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F5" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="G5">
+        <x:v>48000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6">
+      <x:c r="A6" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B6">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C6">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="D6">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E6">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F6" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="G6">
         <x:v>50000</x:v>
       </x:c>
     </x:row>

</xml_diff>